<commit_message>
Get rid of a duplicate
</commit_message>
<xml_diff>
--- a/SI_6_AOP_relevance With Short AOP name.xlsx
+++ b/SI_6_AOP_relevance With Short AOP name.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LADData\RCode\toxEval_Archive\Scripts for Paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LADData\toxManuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D719CAC1-F6EB-42C4-B497-64B9D0CDAA38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SI_AOP_relevance" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="74">
   <si>
     <t>AOP</t>
   </si>
@@ -127,9 +128,6 @@
   </si>
   <si>
     <t>The ToxCast endpoints are relevant to estrogen receptor agonism. The AOP itself is not well developed, but it is likely relevant to vertebrate wildlife and the outcome of altered sexual differentiation is of accepted ecological significance at the population level.</t>
-  </si>
-  <si>
-    <t>The ToxCast endpoints are relevant to estrogen receptor agonism. The AOP links the endpoint response to an effect on survival, and thus an outcome of ecological relevance. However, this AOP is only expected to be relevant at very high and persistent levels of xenoestrogen exposure.</t>
   </si>
   <si>
     <t>The ToxCast endpoints are relevant to estrogen receptor agonism. The AOP links the endpoint response to an effect on survival, and thus and outcome of ecological relevance. However, this AOP is only expected to be relevant at very high and persistent levels of xenoestrogen exposure.</t>
@@ -252,7 +250,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -816,7 +814,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1094,21 +1092,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="87.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="4" max="4" width="87.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>18</v>
       </c>
@@ -1136,10 +1134,10 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>18</v>
       </c>
@@ -1153,10 +1151,10 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19</v>
       </c>
@@ -1170,10 +1168,10 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>77</v>
       </c>
@@ -1184,13 +1182,13 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>77</v>
       </c>
@@ -1201,13 +1199,13 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>77</v>
       </c>
@@ -1218,13 +1216,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>78</v>
       </c>
@@ -1235,13 +1233,13 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>78</v>
       </c>
@@ -1252,13 +1250,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>78</v>
       </c>
@@ -1269,13 +1267,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>79</v>
       </c>
@@ -1286,13 +1284,13 @@
         <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>79</v>
       </c>
@@ -1303,13 +1301,13 @@
         <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>79</v>
       </c>
@@ -1320,13 +1318,13 @@
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>80</v>
       </c>
@@ -1337,13 +1335,13 @@
         <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>80</v>
       </c>
@@ -1354,13 +1352,13 @@
         <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>80</v>
       </c>
@@ -1371,13 +1369,13 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>87</v>
       </c>
@@ -1388,13 +1386,13 @@
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>87</v>
       </c>
@@ -1405,13 +1403,13 @@
         <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>87</v>
       </c>
@@ -1422,13 +1420,13 @@
         <v>15</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>178</v>
       </c>
@@ -1439,13 +1437,13 @@
         <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>178</v>
       </c>
@@ -1456,13 +1454,13 @@
         <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>178</v>
       </c>
@@ -1473,13 +1471,13 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>187</v>
       </c>
@@ -1490,13 +1488,13 @@
         <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>187</v>
       </c>
@@ -1507,13 +1505,13 @@
         <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>187</v>
       </c>
@@ -1524,13 +1522,13 @@
         <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>212</v>
       </c>
@@ -1541,13 +1539,13 @@
         <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>216</v>
       </c>
@@ -1558,13 +1556,13 @@
         <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>238</v>
       </c>
@@ -1575,13 +1573,13 @@
         <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>238</v>
       </c>
@@ -1592,13 +1590,13 @@
         <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>238</v>
       </c>
@@ -1609,13 +1607,13 @@
         <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1623,16 +1621,16 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1640,16 +1638,16 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1657,16 +1655,16 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>8</v>
       </c>
@@ -1674,16 +1672,16 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1691,16 +1689,16 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1708,16 +1706,16 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>11</v>
       </c>
@@ -1725,16 +1723,16 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>12</v>
       </c>
@@ -1742,16 +1740,16 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>13</v>
       </c>
@@ -1759,16 +1757,16 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>17</v>
       </c>
@@ -1776,16 +1774,16 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>26</v>
       </c>
@@ -1793,16 +1791,16 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>26</v>
       </c>
@@ -1810,16 +1808,16 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>26</v>
       </c>
@@ -1827,16 +1825,16 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="75.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>30</v>
       </c>
@@ -1844,16 +1842,16 @@
         <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="75.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>30</v>
       </c>
@@ -1861,16 +1859,16 @@
         <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>34</v>
       </c>
@@ -1878,16 +1876,16 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>34</v>
       </c>
@@ -1895,16 +1893,16 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>34</v>
       </c>
@@ -1912,16 +1910,16 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>34</v>
       </c>
@@ -1929,16 +1927,16 @@
         <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>35</v>
       </c>
@@ -1946,16 +1944,16 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>38</v>
       </c>
@@ -1963,16 +1961,16 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>38</v>
       </c>
@@ -1980,16 +1978,16 @@
         <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>48</v>
       </c>
@@ -1997,16 +1995,16 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>48</v>
       </c>
@@ -2014,16 +2012,16 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="90.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>48</v>
       </c>
@@ -2031,133 +2029,133 @@
         <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <v>57</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>58</v>
       </c>
       <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C57" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E57" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>60</v>
       </c>
       <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C58" t="s">
-        <v>71</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E58" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>111</v>
       </c>
@@ -2165,16 +2163,16 @@
         <v>17</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>112</v>
       </c>
@@ -2182,16 +2180,16 @@
         <v>25</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>112</v>
       </c>
@@ -2199,16 +2197,16 @@
         <v>27</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>130</v>
       </c>
@@ -2216,16 +2214,16 @@
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>130</v>
       </c>
@@ -2233,16 +2231,16 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>130</v>
       </c>
@@ -2250,16 +2248,16 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>144</v>
       </c>
@@ -2267,16 +2265,16 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>144</v>
       </c>
@@ -2284,16 +2282,16 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>144</v>
       </c>
@@ -2301,50 +2299,50 @@
         <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>167</v>
       </c>
@@ -2352,16 +2350,16 @@
         <v>25</v>
       </c>
       <c r="C74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>167</v>
       </c>
@@ -2369,16 +2367,16 @@
         <v>27</v>
       </c>
       <c r="C75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>200</v>
       </c>
@@ -2386,16 +2384,16 @@
         <v>25</v>
       </c>
       <c r="C76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>200</v>
       </c>
@@ -2403,16 +2401,16 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>200</v>
       </c>
@@ -2420,16 +2418,16 @@
         <v>27</v>
       </c>
       <c r="C78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>209</v>
       </c>
@@ -2437,31 +2435,31 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A80" s="2">
         <v>214</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="30.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>217</v>
       </c>
@@ -2469,16 +2467,16 @@
         <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>28</v>
       </c>
@@ -2492,10 +2490,10 @@
         <v>24</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>29</v>
       </c>
@@ -2509,10 +2507,10 @@
         <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>29</v>
       </c>
@@ -2526,10 +2524,10 @@
         <v>26</v>
       </c>
       <c r="E84" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>52</v>
       </c>
@@ -2543,10 +2541,10 @@
         <v>34</v>
       </c>
       <c r="E85" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>52</v>
       </c>
@@ -2560,15 +2558,15 @@
         <v>34</v>
       </c>
       <c r="E86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>53</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
         <v>23</v>
@@ -2577,29 +2575,29 @@
         <v>35</v>
       </c>
       <c r="E87" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B88" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C88" t="s">
         <v>23</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E88" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B89" t="s">
         <v>22</v>
@@ -2608,15 +2606,15 @@
         <v>23</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E89" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B90" t="s">
         <v>22</v>
@@ -2625,15 +2623,15 @@
         <v>23</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E90" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
         <v>22</v>
@@ -2642,15 +2640,15 @@
         <v>23</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B92" t="s">
         <v>22</v>
@@ -2659,69 +2657,69 @@
         <v>23</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E92" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
         <v>23</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E93" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>205</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
         <v>23</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E94" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>205</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E95" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
         <v>23</v>
@@ -2730,63 +2728,46 @@
         <v>55</v>
       </c>
       <c r="E96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>207</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E97" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>207</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C98" t="s">
         <v>23</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E98" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>207</v>
-      </c>
-      <c r="B99" t="s">
-        <v>21</v>
-      </c>
-      <c r="C99" t="s">
-        <v>23</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E99" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E99">
-    <sortCondition ref="C2:C99"/>
+  <sortState ref="A2:E98">
+    <sortCondition ref="C2:C98"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>